<commit_message>
Added update end date feature
</commit_message>
<xml_diff>
--- a/data/packets/vorlage_ZS25.xlsx
+++ b/data/packets/vorlage_ZS25.xlsx
@@ -9,19 +9,25 @@
     <sheet name="Rz" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -45,17 +51,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +401,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -429,8 +428,8 @@
           <t>Auftragsnummer</t>
         </is>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>2210025</v>
+      <c r="B2" t="n">
+        <v>2210024</v>
       </c>
     </row>
     <row r="3">
@@ -439,7 +438,7 @@
           <t>Date_Now</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="1" t="n">
         <v>44885</v>
       </c>
     </row>
@@ -449,7 +448,7 @@
           <t>Time_Now</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="2" t="n">
         <v>0.3007407407407408</v>
       </c>
     </row>
@@ -459,8 +458,8 @@
           <t>Start_Date</t>
         </is>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>44890</v>
+      <c r="B5" s="1" t="n">
+        <v>44859</v>
       </c>
     </row>
     <row r="6">
@@ -469,10 +468,8 @@
           <t>End_Date</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>15-02-2023</t>
-        </is>
+      <c r="B6" s="1" t="n">
+        <v>44946</v>
       </c>
     </row>
     <row r="7">

</xml_diff>